<commit_message>
update to graph drawing
</commit_message>
<xml_diff>
--- a/Properties.xlsx
+++ b/Properties.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Properties</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Graph diameter</t>
+  </si>
+  <si>
+    <t>Avarage clustering coefficient</t>
   </si>
   <si>
     <t>The size of largest component</t>
@@ -398,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,7 +423,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -431,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>287</v>
+        <v>696</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -442,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>600</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -453,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2.0906</v>
+        <v>2.2802</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -464,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.0146</v>
+        <v>0.0066</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -475,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.0018</v>
+        <v>0.0009</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -497,7 +500,18 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>287</v>
+        <v>0.6987</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>